<commit_message>
- latency tests based on gather
</commit_message>
<xml_diff>
--- a/output/arch_comparison.xlsx
+++ b/output/arch_comparison.xlsx
@@ -14,105 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>intel_xeon_6140</t>
-  </si>
-  <si>
-    <t>gather kernel</t>
-  </si>
-  <si>
-    <t>aimed to benchmark L1/LLC/DRAM latency</t>
-  </si>
-  <si>
-    <t>1KB</t>
-  </si>
-  <si>
-    <t>2KB</t>
-  </si>
-  <si>
-    <t>4KB</t>
-  </si>
-  <si>
-    <t>8KB</t>
-  </si>
-  <si>
-    <t>16KB</t>
-  </si>
-  <si>
-    <t>32KB</t>
-  </si>
-  <si>
-    <t>64KB</t>
-  </si>
-  <si>
-    <t>128KB</t>
-  </si>
-  <si>
-    <t>256KB</t>
-  </si>
-  <si>
-    <t>512KB</t>
-  </si>
-  <si>
-    <t>1MB</t>
-  </si>
-  <si>
-    <t>2MB</t>
-  </si>
-  <si>
-    <t>4MB</t>
-  </si>
-  <si>
-    <t>8MB</t>
-  </si>
-  <si>
-    <t>16MB</t>
-  </si>
-  <si>
-    <t>32MB</t>
-  </si>
-  <si>
-    <t>64MB</t>
-  </si>
-  <si>
-    <t>128MB</t>
-  </si>
-  <si>
-    <t>256MB</t>
-  </si>
-  <si>
-    <t>512MB</t>
-  </si>
-  <si>
-    <t>scatter kernel</t>
-  </si>
-  <si>
-    <t>aimed to benchmark ...</t>
-  </si>
-  <si>
-    <t>FMA kernel</t>
-  </si>
-  <si>
-    <t>cpu-bound -&gt; vector-bound -&gt; unit-bound</t>
-  </si>
-  <si>
-    <t>SUSTAINED PERFORMANCE on FLOATS:
- 2067.9 GFLOP/s, 78.1% of peak</t>
-  </si>
-  <si>
-    <t>SUSTAINED PERFORMANCE on DOUBLEs:
- 1038.9 GFLOP/s, 78.7% of peak</t>
-  </si>
-  <si>
-    <t>compute latency kernel</t>
-  </si>
-  <si>
-    <t>cpu-bound -&gt; vector-bound -&gt; latency-bound</t>
-  </si>
-  <si>
-    <t>Performance:
- 174.5 GFLOP/s, 6.6% of peak</t>
   </si>
   <si>
     <t>L1 bandwidth kernel
@@ -155,6 +59,133 @@
  (of theoretical L1 bandwidth 18000)</t>
   </si>
   <si>
+    <t>compute latency kernel
+performs sqrt and fma operations</t>
+  </si>
+  <si>
+    <t>cpu-bound -&gt; vector-bound -&gt; latency-bound</t>
+  </si>
+  <si>
+    <t>Performance:
+ 174.5 GFLOP/s, 6.6% of peak</t>
+  </si>
+  <si>
+    <t>dense vectors kernel (DAXPY)</t>
+  </si>
+  <si>
+    <t>memory-bound -&gt; bandwidth-bound -&gt; DRAM-bound</t>
+  </si>
+  <si>
+    <t>num vectors: 2
+89.1 GB/s, 70.1% of peak</t>
+  </si>
+  <si>
+    <t>num vectors: 2
+89.1 GB/s, 70.2% of peak</t>
+  </si>
+  <si>
+    <t>num vectors: 3
+92.7 GB/s, 73.0% of peak</t>
+  </si>
+  <si>
+    <t>num vectors: 4
+93.0 GB/s, 73.2% of peak</t>
+  </si>
+  <si>
+    <t>num vectors: 5
+116.2 GB/s, 91.5% of peak</t>
+  </si>
+  <si>
+    <t>fibonachi kernel</t>
+  </si>
+  <si>
+    <t>cpu-bound -&gt; scalar-bound -&gt; unit-bound</t>
+  </si>
+  <si>
+    <t>Performance:
+ 50.8 GFLOP/s, 62.0% of peak</t>
+  </si>
+  <si>
+    <t>FMA kernel</t>
+  </si>
+  <si>
+    <t>cpu-bound -&gt; vector-bound -&gt; unit-bound</t>
+  </si>
+  <si>
+    <t>SUSTAINED PERFORMANCE on FLOATS:
+ 2067.9 GFLOP/s, 78.1% of peak</t>
+  </si>
+  <si>
+    <t>SUSTAINED PERFORMANCE on DOUBLEs:
+ 1038.9 GFLOP/s, 78.7% of peak</t>
+  </si>
+  <si>
+    <t>gather kernel</t>
+  </si>
+  <si>
+    <t>aimed to benchmark L1/LLC/DRAM latency</t>
+  </si>
+  <si>
+    <t>1KB</t>
+  </si>
+  <si>
+    <t>2KB</t>
+  </si>
+  <si>
+    <t>4KB</t>
+  </si>
+  <si>
+    <t>8KB</t>
+  </si>
+  <si>
+    <t>16KB</t>
+  </si>
+  <si>
+    <t>32KB</t>
+  </si>
+  <si>
+    <t>64KB</t>
+  </si>
+  <si>
+    <t>128KB</t>
+  </si>
+  <si>
+    <t>256KB</t>
+  </si>
+  <si>
+    <t>512KB</t>
+  </si>
+  <si>
+    <t>1MB</t>
+  </si>
+  <si>
+    <t>2MB</t>
+  </si>
+  <si>
+    <t>4MB</t>
+  </si>
+  <si>
+    <t>8MB</t>
+  </si>
+  <si>
+    <t>16MB</t>
+  </si>
+  <si>
+    <t>32MB</t>
+  </si>
+  <si>
+    <t>64MB</t>
+  </si>
+  <si>
+    <t>128MB</t>
+  </si>
+  <si>
+    <t>256MB</t>
+  </si>
+  <si>
+    <t>512MB</t>
+  </si>
+  <si>
     <t>GEMM algorithm</t>
   </si>
   <si>
@@ -163,6 +194,37 @@
  (of float theoretical peak 2649)</t>
   </si>
   <si>
+    <t>interconnect kernel 
+, performs either local or remote sequential memory accesses</t>
+  </si>
+  <si>
+    <t>memory-bound -&gt; bandwidth-bound -&gt; interconnect-bound</t>
+  </si>
+  <si>
+    <t>mode: one socket accesses local data</t>
+  </si>
+  <si>
+    <t>bandwidth: 74.1 GB/s</t>
+  </si>
+  <si>
+    <t>mode: one socket accesses remote data</t>
+  </si>
+  <si>
+    <t>bandwidth: 35.2 GB/s</t>
+  </si>
+  <si>
+    <t>mode: both sockets access local data</t>
+  </si>
+  <si>
+    <t>bandwidth: 145.2 GB/s</t>
+  </si>
+  <si>
+    <t>mode: both sockets access remote data</t>
+  </si>
+  <si>
+    <t>bandwidth: 51.3 GB/s</t>
+  </si>
+  <si>
     <t>primes algorithm, which detects first N prime numbers. 
 unlike lemher kernel, also has workload balance issues.</t>
   </si>
@@ -175,40 +237,10 @@
  (of theoretical scalar peak 82)</t>
   </si>
   <si>
-    <t>fibonachi kernel</t>
-  </si>
-  <si>
-    <t>cpu-bound -&gt; scalar-bound -&gt; unit-bound</t>
-  </si>
-  <si>
-    <t>Performance:
- 50.8 GFLOP/s, 62.0% of peak</t>
-  </si>
-  <si>
-    <t>dense vectors kernel (DAXPY)</t>
-  </si>
-  <si>
-    <t>memory-bound -&gt; bandwidth-bound -&gt; DRAM-bound</t>
-  </si>
-  <si>
-    <t>num vectors: 2
-89.1 GB/s, 70.1% of peak</t>
-  </si>
-  <si>
-    <t>num vectors: 2
-89.1 GB/s, 70.2% of peak</t>
-  </si>
-  <si>
-    <t>num vectors: 3
-92.7 GB/s, 73.0% of peak</t>
-  </si>
-  <si>
-    <t>num vectors: 4
-93.0 GB/s, 73.2% of peak</t>
-  </si>
-  <si>
-    <t>num vectors: 5
-116.2 GB/s, 91.5% of peak</t>
+    <t>scatter kernel</t>
+  </si>
+  <si>
+    <t>aimed to benchmark ...</t>
   </si>
 </sst>
 </file>
@@ -284,7 +316,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'main_stats'!$C$3:$C$22</c:f>
+              <c:f>'main_stats'!$C$22:$C$41</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -352,7 +384,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'main_stats'!$D$3:$D$22</c:f>
+              <c:f>'main_stats'!$D$22:$D$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -491,7 +523,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'main_stats'!$C$24:$C$43</c:f>
+              <c:f>'main_stats'!$C$52:$C$71</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -559,7 +591,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'main_stats'!$D$24:$D$43</c:f>
+              <c:f>'main_stats'!$D$52:$D$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1022,15 +1054,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="2" max="4" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1038,578 +1069,626 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
-        <v>130</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>134</v>
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>127</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1">
-        <v>134</v>
-      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1">
-        <v>129</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1">
-        <v>129</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1">
-        <v>129</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="1">
-        <v>120</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="1">
-        <v>91</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="1">
-        <v>67</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="1">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1">
-        <v>17</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1">
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1">
-        <v>2</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1">
-        <v>3</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D27" s="1">
-        <v>4</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D28" s="1">
-        <v>5</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D29" s="1">
-        <v>7</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D30" s="1">
-        <v>10</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D31" s="1">
-        <v>15</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1">
-        <v>22</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D33" s="1">
-        <v>28</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1">
-        <v>33</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D35" s="1">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D36" s="1">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D37" s="1">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D38" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="1">
         <v>19</v>
-      </c>
-      <c r="D40" s="1">
-        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D41" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="1">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C43" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" s="1">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:4">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="C52" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="D55" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="D57" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="D59" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" s="1">
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="D61" s="1">
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="D62" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="D63" s="1">
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>42</v>
+      </c>
+      <c r="D64" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="D65" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="D66" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D67" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D71" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A3:A22"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="A24:A43"/>
-    <mergeCell ref="B24:B43"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="A61:A66"/>
-    <mergeCell ref="B61:B66"/>
+  <mergeCells count="10">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A22:A41"/>
+    <mergeCell ref="B22:B41"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="A52:A71"/>
+    <mergeCell ref="B52:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
- bettwer formating - all tests included into analysis table
</commit_message>
<xml_diff>
--- a/output/arch_comparison.xlsx
+++ b/output/arch_comparison.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="206">
   <si>
     <t>intel_xeon_6140</t>
   </si>
@@ -25,6 +25,9 @@
     <t>cpu-bound -&gt; vector-bound -&gt; unit-bound</t>
   </si>
   <si>
+    <t>Performs a sequence of FMA operations.</t>
+  </si>
+  <si>
     <t>float perf:</t>
   </si>
   <si>
@@ -52,7 +55,7 @@
     <t>GEMM algorithm</t>
   </si>
   <si>
-    <t xml:space="preserve">Performs dense matrix-matrix multiplication in single preciesion. </t>
+    <t>Performs dense matrix-matrix multiplication in single preciesion.</t>
   </si>
   <si>
     <t>performance:</t>
@@ -124,44 +127,49 @@
     <t>1.3%</t>
   </si>
   <si>
-    <t>L1 bandwidth kernel
-uses vector instructions to load/store information inside arrays of 16 KB size.
-has multiple modes with instruction level parallelism enabled/disabled.</t>
+    <t>L1 bandwidth kernel</t>
   </si>
   <si>
     <t>memory-bound -&gt; bandwidth-bound -&gt; L1-bound</t>
   </si>
   <si>
-    <t>mode: reads-only, instruction level parallelism available</t>
-  </si>
-  <si>
-    <t>Bandwidth:
- 16217.1 GB/s, 90.1%
- (of theoretical L1 bandwidth 18000)</t>
-  </si>
-  <si>
-    <t>mode: reads and writes, instruction level parallelism available</t>
-  </si>
-  <si>
-    <t>Bandwidth:
- 1421.9 GB/s, 7.9%
- (of theoretical L1 bandwidth 18000)</t>
-  </si>
-  <si>
-    <t>mode: reads-only, no instruction level parallelism available</t>
-  </si>
-  <si>
-    <t>Bandwidth:
- 4587.1 GB/s, 25.5%
- (of theoretical L1 bandwidth 18000)</t>
-  </si>
-  <si>
-    <t>mode: reads-only, array is accessed with random offsets</t>
-  </si>
-  <si>
-    <t>Bandwidth:
- 13854.5 GB/s, 77.0%
- (of theoretical L1 bandwidth 18000)</t>
+    <t>reads-only, instruction level parallelism available</t>
+  </si>
+  <si>
+    <t>bandwidth:</t>
+  </si>
+  <si>
+    <t>reads and writes, instruction level parallelism available</t>
+  </si>
+  <si>
+    <t>reads-only, no instruction level parallelism available</t>
+  </si>
+  <si>
+    <t>reads-only, array is accessed with random offsets</t>
+  </si>
+  <si>
+    <t>16217.1 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>90.1%</t>
+  </si>
+  <si>
+    <t>1421.9 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>7.9%</t>
+  </si>
+  <si>
+    <t>4587.1 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>25.5%</t>
+  </si>
+  <si>
+    <t>13854.5 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>77.0%</t>
   </si>
   <si>
     <t>LLC bandwidth</t>
@@ -170,6 +178,9 @@
     <t>memory-bound -&gt; bandwidth-bound -&gt; LLC-bound</t>
   </si>
   <si>
+    <t xml:space="preserve">multiple operations over </t>
+  </si>
+  <si>
     <t>max bandwidth</t>
   </si>
   <si>
@@ -188,86 +199,115 @@
     <t>15MB</t>
   </si>
   <si>
-    <t>prefix sum</t>
+    <t>prefix sum algorithm</t>
+  </si>
+  <si>
+    <t>Inclusive inplace parallel prefix sum algorithm.</t>
+  </si>
+  <si>
+    <t>93.4 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>16.3%</t>
+  </si>
+  <si>
+    <t>dense vectors kernel</t>
+  </si>
+  <si>
+    <t>memory-bound -&gt; bandwidth-bound -&gt; DRAM-bound</t>
+  </si>
+  <si>
+    <t>2 vectors, copy</t>
+  </si>
+  <si>
+    <t>2 vectors, scale</t>
+  </si>
+  <si>
+    <t>3 vectors, add</t>
+  </si>
+  <si>
+    <t>3 vectors, triada4 vectors, add</t>
+  </si>
+  <si>
+    <t>5 vectors, add</t>
+  </si>
+  <si>
+    <t>88.9 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>70.0%</t>
+  </si>
+  <si>
+    <t>89.1 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>70.1%</t>
+  </si>
+  <si>
+    <t>92.7 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>73.0%</t>
+  </si>
+  <si>
+    <t>92.8 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>92.9 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>73.1%</t>
+  </si>
+  <si>
+    <t>116.3 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>91.6%</t>
+  </si>
+  <si>
+    <t>computing norm algorithm</t>
+  </si>
+  <si>
+    <t>Computing euclidean norm between 2 large vectors (4GB).</t>
+  </si>
+  <si>
+    <t>109.0 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>85.8%</t>
+  </si>
+  <si>
+    <t>interconnect kernel</t>
+  </si>
+  <si>
+    <t>memory-bound -&gt; bandwidth-bound -&gt; interconnect-bound</t>
+  </si>
+  <si>
+    <t>mode: one socket accesses local data</t>
   </si>
   <si>
     <t>bandwidth</t>
   </si>
   <si>
-    <t>93.4 GB/s</t>
-  </si>
-  <si>
-    <t>efficiency</t>
-  </si>
-  <si>
-    <t>16.3%</t>
-  </si>
-  <si>
-    <t>dense vectors kernel (DAXPY)</t>
-  </si>
-  <si>
-    <t>memory-bound -&gt; bandwidth-bound -&gt; DRAM-bound</t>
-  </si>
-  <si>
-    <t>num vectors: 2</t>
-  </si>
-  <si>
-    <t>88.9 GB/s, 70.0%</t>
-  </si>
-  <si>
-    <t>89.1 GB/s, 70.1%</t>
-  </si>
-  <si>
-    <t>num vectors: 3</t>
-  </si>
-  <si>
-    <t>92.7 GB/s, 73.0%</t>
-  </si>
-  <si>
-    <t>92.8 GB/s, 73.0%</t>
-  </si>
-  <si>
-    <t>num vectors: 4</t>
-  </si>
-  <si>
-    <t>92.9 GB/s, 73.1%</t>
-  </si>
-  <si>
-    <t>num vectors: 5</t>
-  </si>
-  <si>
-    <t>116.3 GB/s, 91.6%</t>
-  </si>
-  <si>
-    <t>interconnect kernel 
-, performs either local or remote sequential memory accesses</t>
-  </si>
-  <si>
-    <t>memory-bound -&gt; bandwidth-bound -&gt; interconnect-bound</t>
-  </si>
-  <si>
-    <t>mode: one socket accesses local data</t>
-  </si>
-  <si>
-    <t>bandwidth: 74.1 GB/s</t>
+    <t>74.1 GB/s</t>
   </si>
   <si>
     <t>mode: one socket accesses remote data</t>
   </si>
   <si>
-    <t>bandwidth: 35.3 GB/s</t>
+    <t>35.3 GB/s</t>
   </si>
   <si>
     <t>mode: both sockets access local data</t>
   </si>
   <si>
-    <t>bandwidth: 147.7 GB/s</t>
+    <t>147.7 GB/s</t>
   </si>
   <si>
     <t>mode: both sockets access remote data</t>
   </si>
   <si>
-    <t>bandwidth: 52.1 GB/s</t>
+    <t>52.1 GB/s</t>
   </si>
   <si>
     <t>gather kernel L1 latency</t>
@@ -276,10 +316,28 @@
     <t>memory -&gt; bandwidth -&gt; L1 latency</t>
   </si>
   <si>
-    <t>min bandwidth: 133.643755 GB/s  at 32KB</t>
-  </si>
-  <si>
-    <t>max bandwidth: 137.889919 GB/s  at 9KB</t>
+    <t>Indirectly accessed array is in [1KB, L1 size] range</t>
+  </si>
+  <si>
+    <t>min bandwidth</t>
+  </si>
+  <si>
+    <t>size at which min bandwidth achieved</t>
+  </si>
+  <si>
+    <t>size at which max bandwidth achieved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">133.643755 GB/s </t>
+  </si>
+  <si>
+    <t>32KB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">137.889919 GB/s </t>
+  </si>
+  <si>
+    <t>9KB</t>
   </si>
   <si>
     <t>1KB</t>
@@ -306,9 +364,6 @@
     <t>8KB</t>
   </si>
   <si>
-    <t>9KB</t>
-  </si>
-  <si>
     <t>10KB</t>
   </si>
   <si>
@@ -375,19 +430,22 @@
     <t>31KB</t>
   </si>
   <si>
-    <t>32KB</t>
-  </si>
-  <si>
     <t>gather kernel LLC latency</t>
   </si>
   <si>
     <t>memory -&gt; bandwidth -&gt; LLC latency</t>
   </si>
   <si>
-    <t>min bandwidth: 45.739153 GB/s  at 22MB</t>
-  </si>
-  <si>
-    <t>max bandwidth: 88.647691 GB/s  at 2MB</t>
+    <t>Indirectly accessed array is in [L1/L2 size, LLC size] range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45.739153 GB/s </t>
+  </si>
+  <si>
+    <t>22MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88.647691 GB/s </t>
   </si>
   <si>
     <t>2MB</t>
@@ -447,9 +505,6 @@
     <t>21MB</t>
   </si>
   <si>
-    <t>22MB</t>
-  </si>
-  <si>
     <t>23MB</t>
   </si>
   <si>
@@ -462,10 +517,16 @@
     <t>memory -&gt; bandwidth -&gt; DRAM latency</t>
   </si>
   <si>
-    <t>min bandwidth: 17.656872 GB/s  at 999MB</t>
-  </si>
-  <si>
-    <t>max bandwidth: 33.515301 GB/s  at 49MB</t>
+    <t>Indirectly accessed array is in [LLC size, 2GB] range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.656872 GB/s </t>
+  </si>
+  <si>
+    <t>999MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.515301 GB/s </t>
   </si>
   <si>
     <t>49MB</t>
@@ -525,7 +586,52 @@
     <t>949MB</t>
   </si>
   <si>
-    <t>999MB</t>
+    <t>naive matrix transpose algorithm</t>
+  </si>
+  <si>
+    <t>memory-bound -&gt; latency-bound -&gt; DRAM-bound</t>
+  </si>
+  <si>
+    <t>Simple matrix transpose algorithm. Sequential stores, strided loads.</t>
+  </si>
+  <si>
+    <t>Simple matrix transpose algorithm. Strided stores, sequential loads.</t>
+  </si>
+  <si>
+    <t>25.0 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>19.7%</t>
+  </si>
+  <si>
+    <t>20.5 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>16.1%</t>
+  </si>
+  <si>
+    <t>24.4 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>19.2%</t>
+  </si>
+  <si>
+    <t>22.0 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>17.4%</t>
+  </si>
+  <si>
+    <t>23.2 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>18.3%</t>
+  </si>
+  <si>
+    <t>18.1 GFLOP/s (GIOP/s)</t>
+  </si>
+  <si>
+    <t>14.2%</t>
   </si>
 </sst>
 </file>
@@ -619,7 +725,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'main_stats'!$CY$46:$CY$77</c:f>
+              <c:f>'main_stats'!$CY$57:$CY$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -628,7 +734,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'main_stats'!$CZ$46:$CZ$77</c:f>
+              <c:f>'main_stats'!$CZ$57:$CZ$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -726,92 +832,92 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'main_stats'!$DA$49:$DA$71</c:f>
+              <c:f>'main_stats'!$DA$62:$DA$84</c:f>
               <c:strCache>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>4KB</c:v>
+                  <c:v>6KB</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5KB</c:v>
+                  <c:v>7KB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6KB</c:v>
+                  <c:v>8KB</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7KB</c:v>
+                  <c:v>9KB</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8KB</c:v>
+                  <c:v>10KB</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9KB</c:v>
+                  <c:v>11KB</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10KB</c:v>
+                  <c:v>12KB</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11KB</c:v>
+                  <c:v>13KB</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12KB</c:v>
+                  <c:v>14KB</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13KB</c:v>
+                  <c:v>15KB</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14KB</c:v>
+                  <c:v>16KB</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15KB</c:v>
+                  <c:v>17KB</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16KB</c:v>
+                  <c:v>18KB</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17KB</c:v>
+                  <c:v>19KB</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18KB</c:v>
+                  <c:v>20KB</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19KB</c:v>
+                  <c:v>21KB</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20KB</c:v>
+                  <c:v>22KB</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21KB</c:v>
+                  <c:v>23KB</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22KB</c:v>
+                  <c:v>24KB</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23KB</c:v>
+                  <c:v>25KB</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24KB</c:v>
+                  <c:v>26KB</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>25KB</c:v>
+                  <c:v>27KB</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>26KB</c:v>
+                  <c:v>28KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'main_stats'!$DB$49:$DB$71</c:f>
+              <c:f>'main_stats'!$DB$62:$DB$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>134</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>136</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>137</c:v>
@@ -829,13 +935,13 @@
                   <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>137</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>136</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>137</c:v>
@@ -847,16 +953,16 @@
                   <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>137</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>137</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>136</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>136</c:v>
@@ -865,16 +971,16 @@
                   <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>136</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>135</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>135</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -969,67 +1075,61 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'main_stats'!$DC$52:$DC$71</c:f>
+              <c:f>'main_stats'!$DC$67:$DC$86</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>5MB</c:v>
+                  <c:v>7MB</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6MB</c:v>
+                  <c:v>8MB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7MB</c:v>
+                  <c:v>9MB</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8MB</c:v>
+                  <c:v>10MB</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9MB</c:v>
+                  <c:v>11MB</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10MB</c:v>
+                  <c:v>12MB</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11MB</c:v>
+                  <c:v>13MB</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12MB</c:v>
+                  <c:v>14MB</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13MB</c:v>
+                  <c:v>15MB</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14MB</c:v>
+                  <c:v>16MB</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15MB</c:v>
+                  <c:v>17MB</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16MB</c:v>
+                  <c:v>18MB</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17MB</c:v>
+                  <c:v>19MB</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18MB</c:v>
+                  <c:v>20MB</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19MB</c:v>
+                  <c:v>21MB</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20MB</c:v>
+                  <c:v>22MB</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21MB</c:v>
+                  <c:v>23MB</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22MB</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>23MB</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>24MB</c:v>
                 </c:pt>
               </c:strCache>
@@ -1037,68 +1137,62 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'main_stats'!$DD$52:$DD$71</c:f>
+              <c:f>'main_stats'!$DD$67:$DD$86</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>78</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>73</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>71</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>72</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
@@ -1530,7 +1624,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DF77"/>
+  <dimension ref="A1:DF88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1558,55 +1652,61 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1614,27 +1714,27 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1642,27 +1742,27 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1670,854 +1770,1170 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>47</v>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:5">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E29" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>47</v>
+      <c r="D31" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:5">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="E32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:106">
+    <row r="33" spans="1:5">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:106">
-      <c r="A34" s="1" t="s">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="1" t="s">
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="B35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:106">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:106">
+    <row r="36" spans="1:5">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="1" t="s">
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:106">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="38" spans="1:106">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="D38" s="1" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:106">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:106">
-      <c r="A41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:106">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="D42" s="1" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:106">
+    <row r="43" spans="1:5">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:106">
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D44" s="1" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:106">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:106">
-      <c r="A46" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>82</v>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="DA46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="DB46" s="1">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="47" spans="1:106">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E47" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="E48" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:108">
+      <c r="A49" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="DA47" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="DB47" s="1">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:106">
-      <c r="DA48" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="DB48" s="1">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="49" spans="1:110">
-      <c r="A49" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>118</v>
+      <c r="D49" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="DA49" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="DB49" s="1">
-        <v>134</v>
-      </c>
-      <c r="DC49" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="DD49" s="1">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:110">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:108">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E50" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="DA50" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:108">
+      <c r="A52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="DB50" s="1">
-        <v>136</v>
-      </c>
-      <c r="DC50" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="DD50" s="1">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:110">
-      <c r="DA51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="DB51" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC51" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="DD51" s="1">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="52" spans="1:110">
-      <c r="A52" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="DA52" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="DB52" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC52" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="DD52" s="1">
-        <v>78</v>
-      </c>
-      <c r="DE52" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="DF52" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:110">
+    </row>
+    <row r="53" spans="1:108">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="E53" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="DA53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="DB53" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC53" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="DD53" s="1">
-        <v>77</v>
-      </c>
-      <c r="DE53" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="DF53" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:110">
-      <c r="DA54" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="DB54" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC54" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="DD54" s="1">
-        <v>76</v>
-      </c>
-      <c r="DE54" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="DF54" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="1:110">
-      <c r="DA55" s="1" t="s">
+    </row>
+    <row r="54" spans="1:108">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="DB55" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC55" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="DD55" s="1">
-        <v>75</v>
-      </c>
-      <c r="DE55" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="DF55" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="1:110">
-      <c r="DA56" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="DB56" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC56" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="DD56" s="1">
-        <v>75</v>
-      </c>
-      <c r="DE56" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="DF56" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:110">
+    </row>
+    <row r="55" spans="1:108">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:108">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:108">
+      <c r="A57" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="DA57" s="1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="DB57" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC57" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="DD57" s="1">
-        <v>74</v>
-      </c>
-      <c r="DE57" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="DF57" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:110">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:108">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="DA58" s="1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="DB58" s="1">
         <v>136</v>
       </c>
-      <c r="DC58" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DD58" s="1">
-        <v>74</v>
-      </c>
-      <c r="DE58" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="DF58" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:110">
+    </row>
+    <row r="59" spans="1:108">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="DA59" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="DB59" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC59" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="DD59" s="1">
-        <v>74</v>
-      </c>
-      <c r="DE59" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="DF59" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:110">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:108">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="DA60" s="1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="DB60" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC60" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="DD60" s="1">
-        <v>73</v>
-      </c>
-      <c r="DE60" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="DF60" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="1:110">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:108">
       <c r="DA61" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="DB61" s="1">
-        <v>137</v>
-      </c>
-      <c r="DC61" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="DD61" s="1">
-        <v>71</v>
-      </c>
-      <c r="DE61" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="DF61" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:110">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:108">
+      <c r="A62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="DA62" s="1" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="DB62" s="1">
         <v>137</v>
       </c>
       <c r="DC62" s="1" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="DD62" s="1">
-        <v>72</v>
-      </c>
-      <c r="DE62" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="DF62" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="1:110">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:108">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="DA63" s="1" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="DB63" s="1">
         <v>137</v>
       </c>
       <c r="DC63" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="DD63" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:108">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DA64" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DB64" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC64" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="DD64" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:110">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="DA65" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DB65" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC65" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="DD65" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:110">
+      <c r="DA66" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DB66" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC66" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="DD66" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="1:110">
+      <c r="A67" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="DA67" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DB67" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC67" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD67" s="1">
+        <v>76</v>
+      </c>
+      <c r="DE67" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="DF67" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:110">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="DA68" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DB68" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC68" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="DD68" s="1">
+        <v>75</v>
+      </c>
+      <c r="DE68" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="DF68" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:110">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="DA69" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DB69" s="1">
+        <v>136</v>
+      </c>
+      <c r="DC69" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DD69" s="1">
+        <v>75</v>
+      </c>
+      <c r="DE69" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="DF69" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:110">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="DA70" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DB70" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC70" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DD70" s="1">
+        <v>74</v>
+      </c>
+      <c r="DE70" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="DF70" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:110">
+      <c r="DA71" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DB71" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC71" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DD71" s="1">
+        <v>74</v>
+      </c>
+      <c r="DE71" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="DF71" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:110">
+      <c r="A72" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="DA72" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DB72" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC72" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="DD72" s="1">
+        <v>74</v>
+      </c>
+      <c r="DE72" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="DF72" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:110">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="DA73" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DB73" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC73" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="DD73" s="1">
+        <v>73</v>
+      </c>
+      <c r="DE73" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="DF73" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:110">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="DA74" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DB74" s="1">
+        <v>137</v>
+      </c>
+      <c r="DC74" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DD74" s="1">
+        <v>71</v>
+      </c>
+      <c r="DE74" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="DF74" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:110">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="DA75" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DB75" s="1">
+        <v>136</v>
+      </c>
+      <c r="DC75" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="DD75" s="1">
+        <v>72</v>
+      </c>
+      <c r="DE75" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="DF75" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:110">
+      <c r="E76" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="DA76" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DB76" s="1">
+        <v>136</v>
+      </c>
+      <c r="DC76" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="DD76" s="1">
+        <v>63</v>
+      </c>
+      <c r="DE76" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="DF76" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:110">
+      <c r="E77" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="DA77" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DB77" s="1">
+        <v>136</v>
+      </c>
+      <c r="DC77" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="DD77" s="1">
+        <v>70</v>
+      </c>
+      <c r="DE77" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="DF77" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:110">
+      <c r="E78" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="DA78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DB78" s="1">
+        <v>135</v>
+      </c>
+      <c r="DC78" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="DD78" s="1">
+        <v>72</v>
+      </c>
+      <c r="DE78" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="DF78" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:110">
+      <c r="E79" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DA79" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="DB79" s="1">
+        <v>136</v>
+      </c>
+      <c r="DC79" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="DD79" s="1">
+        <v>71</v>
+      </c>
+      <c r="DE79" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="DF79" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:110">
+      <c r="E80" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="DA80" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="DB80" s="1">
+        <v>135</v>
+      </c>
+      <c r="DC80" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="DD80" s="1">
+        <v>72</v>
+      </c>
+      <c r="DE80" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="DF80" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="5:110">
+      <c r="E81" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="DA81" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="DB81" s="1">
+        <v>135</v>
+      </c>
+      <c r="DC81" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="DD81" s="1">
+        <v>54</v>
+      </c>
+      <c r="DE81" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="DF81" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="5:110">
+      <c r="E82" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="DA82" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DB82" s="1">
+        <v>135</v>
+      </c>
+      <c r="DC82" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="DD82" s="1">
+        <v>45</v>
+      </c>
+      <c r="DE82" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="DF82" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="5:110">
+      <c r="E83" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="DA83" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DB83" s="1">
         <v>134</v>
       </c>
-      <c r="DD63" s="1">
-        <v>63</v>
-      </c>
-      <c r="DE63" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="DF63" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="64" spans="1:110">
-      <c r="DA64" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="DB64" s="1">
+      <c r="DC83" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="DD83" s="1">
+        <v>61</v>
+      </c>
+      <c r="DE83" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="DF83" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="5:110">
+      <c r="DA84" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DB84" s="1">
+        <v>134</v>
+      </c>
+      <c r="DC84" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="DD84" s="1">
+        <v>65</v>
+      </c>
+      <c r="DE84" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="DF84" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="5:110">
+      <c r="DA85" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="DB85" s="1">
+        <v>134</v>
+      </c>
+      <c r="DE85" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="DF85" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="5:110">
+      <c r="DA86" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="DC64" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="DD64" s="1">
-        <v>70</v>
-      </c>
-      <c r="DE64" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="DF64" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="105:110">
-      <c r="DA65" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="DB65" s="1">
-        <v>136</v>
-      </c>
-      <c r="DC65" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="DD65" s="1">
-        <v>72</v>
-      </c>
-      <c r="DE65" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="DF65" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="105:110">
-      <c r="DA66" s="1" t="s">
+      <c r="DB86" s="1">
+        <v>134</v>
+      </c>
+      <c r="DE86" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="DF86" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="5:110">
+      <c r="DA87" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="DB87" s="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="5:110">
+      <c r="DA88" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DB66" s="1">
-        <v>136</v>
-      </c>
-      <c r="DC66" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="DD66" s="1">
-        <v>71</v>
-      </c>
-      <c r="DE66" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="DF66" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="105:110">
-      <c r="DA67" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="DB67" s="1">
-        <v>135</v>
-      </c>
-      <c r="DC67" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="DD67" s="1">
-        <v>72</v>
-      </c>
-      <c r="DE67" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="DF67" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="105:110">
-      <c r="DA68" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="DB68" s="1">
-        <v>136</v>
-      </c>
-      <c r="DC68" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="DD68" s="1">
-        <v>54</v>
-      </c>
-      <c r="DE68" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="DF68" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="105:110">
-      <c r="DA69" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="DB69" s="1">
-        <v>135</v>
-      </c>
-      <c r="DC69" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="DD69" s="1">
-        <v>45</v>
-      </c>
-      <c r="DE69" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="DF69" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="105:110">
-      <c r="DA70" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="DB70" s="1">
-        <v>135</v>
-      </c>
-      <c r="DC70" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="DD70" s="1">
-        <v>61</v>
-      </c>
-      <c r="DE70" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="DF70" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="105:110">
-      <c r="DA71" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="DB71" s="1">
-        <v>135</v>
-      </c>
-      <c r="DC71" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="DD71" s="1">
-        <v>65</v>
-      </c>
-      <c r="DE71" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="DF71" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="105:110">
-      <c r="DA72" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="DB72" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="73" spans="105:110">
-      <c r="DA73" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="DB73" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="74" spans="105:110">
-      <c r="DA74" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="DB74" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="75" spans="105:110">
-      <c r="DA75" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="DB75" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="76" spans="105:110">
-      <c r="DA76" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="DB76" s="1">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="77" spans="105:110">
-      <c r="DA77" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="DB77" s="1">
+      <c r="DB88" s="1">
         <v>133</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="55">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
@@ -2533,22 +2949,43 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A22:A29"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A38:A47"/>
+    <mergeCell ref="B38:B47"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:C47"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C74:C75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
- generic compute latency
</commit_message>
<xml_diff>
--- a/output/arch_comparison.xlsx
+++ b/output/arch_comparison.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="378">
   <si>
     <t>intel_xeon_6140</t>
   </si>
@@ -689,6 +689,465 @@
   </si>
   <si>
     <t xml:space="preserve">80.138276 MTEPS </t>
+  </si>
+  <si>
+    <t>kunpeng_920_64_core</t>
+  </si>
+  <si>
+    <t>443.7 GFLOP/s</t>
+  </si>
+  <si>
+    <t>33.3%</t>
+  </si>
+  <si>
+    <t>507.8 GFLOP/s</t>
+  </si>
+  <si>
+    <t>76.9%</t>
+  </si>
+  <si>
+    <t>5034340659.3 GFLOP/s</t>
+  </si>
+  <si>
+    <t>378237465.0%</t>
+  </si>
+  <si>
+    <t>360.6 GFLOP/s</t>
+  </si>
+  <si>
+    <t>27.1%</t>
+  </si>
+  <si>
+    <t>166.2 GFLOP/s</t>
+  </si>
+  <si>
+    <t>50.1%</t>
+  </si>
+  <si>
+    <t>1040.2 GFLOP/s</t>
+  </si>
+  <si>
+    <t>313.3%</t>
+  </si>
+  <si>
+    <t>27.6 GFLOP/s</t>
+  </si>
+  <si>
+    <t>8.3%</t>
+  </si>
+  <si>
+    <t>58.0 GFLOP/s</t>
+  </si>
+  <si>
+    <t>17.5%</t>
+  </si>
+  <si>
+    <t>14.1 GFLOP/s</t>
+  </si>
+  <si>
+    <t>4613.2 GB/s</t>
+  </si>
+  <si>
+    <t>61.5%</t>
+  </si>
+  <si>
+    <t>6806.5 GB/s</t>
+  </si>
+  <si>
+    <t>90.8%</t>
+  </si>
+  <si>
+    <t>1915.1 GB/s</t>
+  </si>
+  <si>
+    <t>2354.9 GB/s</t>
+  </si>
+  <si>
+    <t>31.4%</t>
+  </si>
+  <si>
+    <t>888.8 GB/s</t>
+  </si>
+  <si>
+    <t>63.6%</t>
+  </si>
+  <si>
+    <t>38MB</t>
+  </si>
+  <si>
+    <t>157.0 GB/s</t>
+  </si>
+  <si>
+    <t>11.2%</t>
+  </si>
+  <si>
+    <t>114.7 GB/s</t>
+  </si>
+  <si>
+    <t>61.4%</t>
+  </si>
+  <si>
+    <t>112.2 GB/s</t>
+  </si>
+  <si>
+    <t>60.0%</t>
+  </si>
+  <si>
+    <t>122.0 GB/s</t>
+  </si>
+  <si>
+    <t>65.2%</t>
+  </si>
+  <si>
+    <t>119.3 GB/s</t>
+  </si>
+  <si>
+    <t>63.8%</t>
+  </si>
+  <si>
+    <t>108.4 GB/s</t>
+  </si>
+  <si>
+    <t>58.0%</t>
+  </si>
+  <si>
+    <t>155.3 GB/s</t>
+  </si>
+  <si>
+    <t>83.1%</t>
+  </si>
+  <si>
+    <t>101.6 GB/s</t>
+  </si>
+  <si>
+    <t>54.3%</t>
+  </si>
+  <si>
+    <t>65.5 GB/s</t>
+  </si>
+  <si>
+    <t>72.5 GB/s</t>
+  </si>
+  <si>
+    <t>138.9 GB/s</t>
+  </si>
+  <si>
+    <t>61.0 GB/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">129.46761 GB/s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">200.812727 GB/s </t>
+  </si>
+  <si>
+    <t>37KB</t>
+  </si>
+  <si>
+    <t>33KB</t>
+  </si>
+  <si>
+    <t>34KB</t>
+  </si>
+  <si>
+    <t>35KB</t>
+  </si>
+  <si>
+    <t>36KB</t>
+  </si>
+  <si>
+    <t>38KB</t>
+  </si>
+  <si>
+    <t>39KB</t>
+  </si>
+  <si>
+    <t>40KB</t>
+  </si>
+  <si>
+    <t>41KB</t>
+  </si>
+  <si>
+    <t>42KB</t>
+  </si>
+  <si>
+    <t>43KB</t>
+  </si>
+  <si>
+    <t>44KB</t>
+  </si>
+  <si>
+    <t>45KB</t>
+  </si>
+  <si>
+    <t>46KB</t>
+  </si>
+  <si>
+    <t>47KB</t>
+  </si>
+  <si>
+    <t>48KB</t>
+  </si>
+  <si>
+    <t>49KB</t>
+  </si>
+  <si>
+    <t>50KB</t>
+  </si>
+  <si>
+    <t>51KB</t>
+  </si>
+  <si>
+    <t>52KB</t>
+  </si>
+  <si>
+    <t>53KB</t>
+  </si>
+  <si>
+    <t>54KB</t>
+  </si>
+  <si>
+    <t>55KB</t>
+  </si>
+  <si>
+    <t>56KB</t>
+  </si>
+  <si>
+    <t>57KB</t>
+  </si>
+  <si>
+    <t>58KB</t>
+  </si>
+  <si>
+    <t>59KB</t>
+  </si>
+  <si>
+    <t>60KB</t>
+  </si>
+  <si>
+    <t>61KB</t>
+  </si>
+  <si>
+    <t>62KB</t>
+  </si>
+  <si>
+    <t>63KB</t>
+  </si>
+  <si>
+    <t>64KB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.222691 MTEPS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.866183 GB/s </t>
+  </si>
+  <si>
+    <t>40MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109.187606 GB/s </t>
+  </si>
+  <si>
+    <t>1MB</t>
+  </si>
+  <si>
+    <t>25MB</t>
+  </si>
+  <si>
+    <t>26MB</t>
+  </si>
+  <si>
+    <t>27MB</t>
+  </si>
+  <si>
+    <t>28MB</t>
+  </si>
+  <si>
+    <t>29MB</t>
+  </si>
+  <si>
+    <t>30MB</t>
+  </si>
+  <si>
+    <t>31MB</t>
+  </si>
+  <si>
+    <t>32MB</t>
+  </si>
+  <si>
+    <t>33MB</t>
+  </si>
+  <si>
+    <t>34MB</t>
+  </si>
+  <si>
+    <t>35MB</t>
+  </si>
+  <si>
+    <t>36MB</t>
+  </si>
+  <si>
+    <t>37MB</t>
+  </si>
+  <si>
+    <t>39MB</t>
+  </si>
+  <si>
+    <t>41MB</t>
+  </si>
+  <si>
+    <t>42MB</t>
+  </si>
+  <si>
+    <t>43MB</t>
+  </si>
+  <si>
+    <t>44MB</t>
+  </si>
+  <si>
+    <t>45MB</t>
+  </si>
+  <si>
+    <t>46MB</t>
+  </si>
+  <si>
+    <t>47MB</t>
+  </si>
+  <si>
+    <t>49MB</t>
+  </si>
+  <si>
+    <t>50MB</t>
+  </si>
+  <si>
+    <t>51MB</t>
+  </si>
+  <si>
+    <t>52MB</t>
+  </si>
+  <si>
+    <t>53MB</t>
+  </si>
+  <si>
+    <t>54MB</t>
+  </si>
+  <si>
+    <t>55MB</t>
+  </si>
+  <si>
+    <t>56MB</t>
+  </si>
+  <si>
+    <t>57MB</t>
+  </si>
+  <si>
+    <t>58MB</t>
+  </si>
+  <si>
+    <t>59MB</t>
+  </si>
+  <si>
+    <t>60MB</t>
+  </si>
+  <si>
+    <t>61MB</t>
+  </si>
+  <si>
+    <t>62MB</t>
+  </si>
+  <si>
+    <t>63MB</t>
+  </si>
+  <si>
+    <t>64MB</t>
+  </si>
+  <si>
+    <t>65MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">197.527539 MTEPS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.710487 GB/s </t>
+  </si>
+  <si>
+    <t>980MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.974432 GB/s </t>
+  </si>
+  <si>
+    <t>130MB</t>
+  </si>
+  <si>
+    <t>180MB</t>
+  </si>
+  <si>
+    <t>230MB</t>
+  </si>
+  <si>
+    <t>280MB</t>
+  </si>
+  <si>
+    <t>330MB</t>
+  </si>
+  <si>
+    <t>380MB</t>
+  </si>
+  <si>
+    <t>430MB</t>
+  </si>
+  <si>
+    <t>480MB</t>
+  </si>
+  <si>
+    <t>530MB</t>
+  </si>
+  <si>
+    <t>580MB</t>
+  </si>
+  <si>
+    <t>630MB</t>
+  </si>
+  <si>
+    <t>680MB</t>
+  </si>
+  <si>
+    <t>730MB</t>
+  </si>
+  <si>
+    <t>780MB</t>
+  </si>
+  <si>
+    <t>830MB</t>
+  </si>
+  <si>
+    <t>880MB</t>
+  </si>
+  <si>
+    <t>930MB</t>
+  </si>
+  <si>
+    <t>9.4 GB/s</t>
+  </si>
+  <si>
+    <t>5.0%</t>
+  </si>
+  <si>
+    <t>5.6 GB/s</t>
+  </si>
+  <si>
+    <t>3.0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41.018904 MTEPS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">54.597663 MTEPS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.426875 MTEPS </t>
   </si>
 </sst>
 </file>
@@ -773,7 +1232,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="12900D"/>
+                <a:srgbClr val="9F8511"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -782,9 +1241,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'main_stats'!$DU$65:$DU$96</c:f>
+              <c:f>'main_stats'!$DU$65:$DU$128</c:f>
               <c:strCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="64"/>
                 <c:pt idx="0">
                   <c:v>1KB</c:v>
                 </c:pt>
@@ -886,10 +1345,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'main_stats'!$DV$65:$DV$96</c:f>
+              <c:f>'main_stats'!$DV$65:$DV$128</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="64"/>
                 <c:pt idx="0">
                   <c:v>140</c:v>
                 </c:pt>
@@ -985,6 +1444,424 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>137</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>kunpeng_920_64_core</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="E6DA22"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'main_stats'!$EA$65:$EA$128</c:f>
+              <c:strCache>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>1KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5KB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6KB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17KB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18KB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19KB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20KB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21KB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22KB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23KB</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24KB</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25KB</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26KB</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27KB</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28KB</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29KB</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30KB</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31KB</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32KB</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33KB</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34KB</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35KB</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36KB</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37KB</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38KB</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39KB</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40KB</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41KB</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42KB</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43KB</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44KB</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45KB</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46KB</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47KB</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48KB</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49KB</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50KB</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51KB</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52KB</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53KB</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54KB</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55KB</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56KB</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57KB</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58KB</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59KB</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60KB</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61KB</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62KB</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63KB</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'main_stats'!$EB$65:$EB$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1070,7 +1947,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="3210BF"/>
+                <a:srgbClr val="556652"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1079,9 +1956,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'main_stats'!$DW$72:$DW$94</c:f>
+              <c:f>'main_stats'!$DW$72:$DW$136</c:f>
               <c:strCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>2MB</c:v>
                 </c:pt>
@@ -1156,10 +2033,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'main_stats'!$DX$72:$DX$94</c:f>
+              <c:f>'main_stats'!$DX$72:$DX$136</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>88</c:v>
                 </c:pt>
@@ -1228,6 +2105,430 @@
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>kunpeng_920_64_core</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="D1E2EC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'main_stats'!$EC$72:$EC$136</c:f>
+              <c:strCache>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>1MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3MB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4MB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5MB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6MB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7MB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8MB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9MB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10MB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11MB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12MB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13MB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14MB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15MB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16MB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23MB</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24MB</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25MB</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26MB</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27MB</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28MB</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29MB</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30MB</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31MB</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32MB</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33MB</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34MB</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35MB</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36MB</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37MB</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38MB</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39MB</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40MB</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41MB</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42MB</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43MB</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44MB</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45MB</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46MB</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47MB</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48MB</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49MB</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50MB</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51MB</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52MB</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53MB</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54MB</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55MB</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56MB</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57MB</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58MB</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59MB</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60MB</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61MB</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62MB</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63MB</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64MB</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'main_stats'!$ED$72:$ED$136</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1313,7 +2614,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="DAE90B"/>
+                <a:srgbClr val="226A4A"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1453,6 +2754,148 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>kunpeng_920_64_core</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="DD9DC2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'main_stats'!$EE$79:$EE$98</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>130MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230MB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>280MB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>330MB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>380MB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>430MB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>480MB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>530MB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>580MB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>630MB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>680MB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>730MB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>780MB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>830MB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>880MB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>930MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>980MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'main_stats'!$EF$79:$EF$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1883,7 +3326,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DZ98"/>
+  <dimension ref="A1:EF136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1894,14 +3337,18 @@
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="E1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1917,8 +3364,11 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1928,8 +3378,11 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1939,8 +3392,11 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1950,8 +3406,11 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F5" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1967,8 +3426,11 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1978,8 +3440,11 @@
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F8" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1995,8 +3460,11 @@
       <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2006,8 +3474,11 @@
       <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F11" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2023,8 +3494,11 @@
       <c r="E13" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2034,8 +3508,11 @@
       <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F14" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -2051,8 +3528,11 @@
       <c r="E16" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2062,8 +3542,11 @@
       <c r="E17" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F17" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -2079,8 +3562,11 @@
       <c r="E19" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2090,8 +3576,11 @@
       <c r="E20" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F20" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -2107,8 +3596,11 @@
       <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2118,8 +3610,11 @@
       <c r="E23" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F23" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -2135,8 +3630,11 @@
       <c r="E25" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2146,8 +3644,11 @@
       <c r="E26" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>45</v>
       </c>
@@ -2163,8 +3664,11 @@
       <c r="E28" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2174,8 +3678,11 @@
       <c r="E29" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
@@ -2187,8 +3694,11 @@
       <c r="E30" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2198,8 +3708,11 @@
       <c r="E31" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -2211,8 +3724,11 @@
       <c r="E32" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2222,8 +3738,11 @@
       <c r="E33" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -2235,8 +3754,11 @@
       <c r="E34" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2246,8 +3768,11 @@
       <c r="E35" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F35" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -2263,8 +3788,11 @@
       <c r="E37" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2274,8 +3802,11 @@
       <c r="E38" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2285,13 +3816,16 @@
       <c r="E39" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
         <v>69</v>
       </c>
@@ -2307,8 +3841,11 @@
       <c r="E41" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2318,8 +3855,11 @@
       <c r="E42" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F42" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
         <v>73</v>
       </c>
@@ -2335,8 +3875,11 @@
       <c r="E44" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2346,8 +3889,11 @@
       <c r="E45" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
@@ -2359,8 +3905,11 @@
       <c r="E46" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2370,8 +3919,11 @@
       <c r="E47" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
@@ -2383,8 +3935,11 @@
       <c r="E48" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2394,8 +3949,11 @@
       <c r="E49" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -2407,8 +3965,11 @@
       <c r="E50" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2418,8 +3979,11 @@
       <c r="E51" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
@@ -2431,8 +3995,11 @@
       <c r="E52" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2442,8 +4009,11 @@
       <c r="E53" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
@@ -2455,8 +4025,11 @@
       <c r="E54" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2466,8 +4039,11 @@
       <c r="E55" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F55" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
         <v>92</v>
       </c>
@@ -2483,8 +4059,11 @@
       <c r="E57" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2494,8 +4073,11 @@
       <c r="E58" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F58" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="1" t="s">
         <v>96</v>
       </c>
@@ -2511,8 +4093,11 @@
       <c r="E60" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
@@ -2524,8 +4109,11 @@
       <c r="E61" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -2537,8 +4125,11 @@
       <c r="E62" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
@@ -2550,12 +4141,15 @@
       <c r="E63" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="1:130">
+    <row r="65" spans="1:136">
       <c r="A65" s="1" t="s">
         <v>107</v>
       </c>
@@ -2571,14 +4165,23 @@
       <c r="E65" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="F65" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="DU65" s="1" t="s">
         <v>117</v>
       </c>
       <c r="DV65" s="1">
         <v>140</v>
       </c>
-    </row>
-    <row r="66" spans="1:130">
+      <c r="EA65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="EB65" s="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:136">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2588,14 +4191,23 @@
       <c r="E66" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="F66" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="DU66" s="1" t="s">
         <v>118</v>
       </c>
       <c r="DV66" s="1">
         <v>140</v>
       </c>
-    </row>
-    <row r="67" spans="1:130">
+      <c r="EA66" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="EB66" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:136">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2605,14 +4217,23 @@
       <c r="E67" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="F67" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="DU67" s="1" t="s">
         <v>119</v>
       </c>
       <c r="DV67" s="1">
         <v>136</v>
       </c>
-    </row>
-    <row r="68" spans="1:130">
+      <c r="EA67" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="EB67" s="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:136">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2622,22 +4243,37 @@
       <c r="E68" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="F68" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="DU68" s="1" t="s">
         <v>120</v>
       </c>
       <c r="DV68" s="1">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:130">
+      <c r="EA68" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="EB68" s="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:136">
       <c r="DU69" s="1" t="s">
         <v>121</v>
       </c>
       <c r="DV69" s="1">
         <v>140</v>
       </c>
-    </row>
-    <row r="70" spans="1:130">
+      <c r="EA69" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="EB69" s="1">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="70" spans="1:136">
       <c r="A70" s="1" t="s">
         <v>147</v>
       </c>
@@ -2653,22 +4289,37 @@
       <c r="E70" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="F70" s="1" t="s">
+        <v>307</v>
+      </c>
       <c r="DU70" s="1" t="s">
         <v>122</v>
       </c>
       <c r="DV70" s="1">
         <v>140</v>
       </c>
-    </row>
-    <row r="71" spans="1:130">
+      <c r="EA70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="EB70" s="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:136">
       <c r="DU71" s="1" t="s">
         <v>123</v>
       </c>
       <c r="DV71" s="1">
         <v>140</v>
       </c>
-    </row>
-    <row r="72" spans="1:130">
+      <c r="EA71" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="EB71" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:136">
       <c r="A72" s="1" t="s">
         <v>152</v>
       </c>
@@ -2684,6 +4335,9 @@
       <c r="E72" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="F72" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="DU72" s="1" t="s">
         <v>124</v>
       </c>
@@ -2696,8 +4350,20 @@
       <c r="DX72" s="1">
         <v>88</v>
       </c>
-    </row>
-    <row r="73" spans="1:130">
+      <c r="EA72" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EB72" s="1">
+        <v>140</v>
+      </c>
+      <c r="EC72" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="ED72" s="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:136">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2707,6 +4373,9 @@
       <c r="E73" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="F73" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="DU73" s="1" t="s">
         <v>116</v>
       </c>
@@ -2719,8 +4388,20 @@
       <c r="DX73" s="1">
         <v>82</v>
       </c>
-    </row>
-    <row r="74" spans="1:130">
+      <c r="EA73" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="EB73" s="1">
+        <v>137</v>
+      </c>
+      <c r="EC73" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="ED73" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:136">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2730,6 +4411,9 @@
       <c r="E74" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="F74" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="DU74" s="1" t="s">
         <v>125</v>
       </c>
@@ -2742,8 +4426,20 @@
       <c r="DX74" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="75" spans="1:130">
+      <c r="EA74" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="EB74" s="1">
+        <v>151</v>
+      </c>
+      <c r="EC74" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="ED74" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:136">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2753,6 +4449,9 @@
       <c r="E75" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="F75" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="DU75" s="1" t="s">
         <v>126</v>
       </c>
@@ -2765,8 +4464,20 @@
       <c r="DX75" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="76" spans="1:130">
+      <c r="EA75" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="EB75" s="1">
+        <v>135</v>
+      </c>
+      <c r="EC75" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="ED75" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:136">
       <c r="DU76" s="1" t="s">
         <v>127</v>
       </c>
@@ -2779,8 +4490,20 @@
       <c r="DX76" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="77" spans="1:130">
+      <c r="EA76" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="EB76" s="1">
+        <v>132</v>
+      </c>
+      <c r="EC76" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="ED76" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:136">
       <c r="A77" s="1" t="s">
         <v>179</v>
       </c>
@@ -2796,6 +4519,9 @@
       <c r="E77" s="1" t="s">
         <v>182</v>
       </c>
+      <c r="F77" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="DU77" s="1" t="s">
         <v>128</v>
       </c>
@@ -2808,8 +4534,20 @@
       <c r="DX77" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:130">
+      <c r="EA77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="EB77" s="1">
+        <v>150</v>
+      </c>
+      <c r="EC77" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="ED77" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="1:136">
       <c r="DU78" s="1" t="s">
         <v>129</v>
       </c>
@@ -2822,8 +4560,20 @@
       <c r="DX78" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:130">
+      <c r="EA78" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="EB78" s="1">
+        <v>157</v>
+      </c>
+      <c r="EC78" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="ED78" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="1:136">
       <c r="A79" s="1" t="s">
         <v>183</v>
       </c>
@@ -2839,6 +4589,9 @@
       <c r="E79" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="F79" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="DU79" s="1" t="s">
         <v>130</v>
       </c>
@@ -2857,8 +4610,26 @@
       <c r="DZ79" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="80" spans="1:130">
+      <c r="EA79" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="EB79" s="1">
+        <v>158</v>
+      </c>
+      <c r="EC79" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="ED79" s="1">
+        <v>57</v>
+      </c>
+      <c r="EE79" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="EF79" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:136">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2868,6 +4639,9 @@
       <c r="E80" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="F80" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="DU80" s="1" t="s">
         <v>131</v>
       </c>
@@ -2886,8 +4660,26 @@
       <c r="DZ80" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="81" spans="1:130">
+      <c r="EA80" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="EB80" s="1">
+        <v>133</v>
+      </c>
+      <c r="EC80" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="ED80" s="1">
+        <v>47</v>
+      </c>
+      <c r="EE80" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="EF80" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:136">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2897,6 +4689,9 @@
       <c r="E81" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="F81" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="DU81" s="1" t="s">
         <v>132</v>
       </c>
@@ -2915,8 +4710,26 @@
       <c r="DZ81" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="82" spans="1:130">
+      <c r="EA81" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="EB81" s="1">
+        <v>198</v>
+      </c>
+      <c r="EC81" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="ED81" s="1">
+        <v>47</v>
+      </c>
+      <c r="EE81" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="EF81" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:136">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2926,6 +4739,9 @@
       <c r="E82" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="F82" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="DU82" s="1" t="s">
         <v>133</v>
       </c>
@@ -2944,8 +4760,26 @@
       <c r="DZ82" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="83" spans="1:130">
+      <c r="EA82" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="EB82" s="1">
+        <v>138</v>
+      </c>
+      <c r="EC82" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="ED82" s="1">
+        <v>44</v>
+      </c>
+      <c r="EE82" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="EF82" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:136">
       <c r="DU83" s="1" t="s">
         <v>134</v>
       </c>
@@ -2964,8 +4798,26 @@
       <c r="DZ83" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="84" spans="1:130">
+      <c r="EA83" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="EB83" s="1">
+        <v>134</v>
+      </c>
+      <c r="EC83" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="ED83" s="1">
+        <v>43</v>
+      </c>
+      <c r="EE83" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="EF83" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:136">
       <c r="A84" s="1" t="s">
         <v>208</v>
       </c>
@@ -2981,6 +4833,9 @@
       <c r="E84" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="F84" s="1" t="s">
+        <v>371</v>
+      </c>
       <c r="DU84" s="1" t="s">
         <v>135</v>
       </c>
@@ -2999,8 +4854,26 @@
       <c r="DZ84" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="85" spans="1:130">
+      <c r="EA84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="EB84" s="1">
+        <v>151</v>
+      </c>
+      <c r="EC84" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="ED84" s="1">
+        <v>42</v>
+      </c>
+      <c r="EE84" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="EF84" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:136">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -3010,6 +4883,9 @@
       <c r="E85" s="1" t="s">
         <v>213</v>
       </c>
+      <c r="F85" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="DU85" s="1" t="s">
         <v>136</v>
       </c>
@@ -3028,8 +4904,26 @@
       <c r="DZ85" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="86" spans="1:130">
+      <c r="EA85" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EB85" s="1">
+        <v>189</v>
+      </c>
+      <c r="EC85" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="ED85" s="1">
+        <v>41</v>
+      </c>
+      <c r="EE85" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="EF85" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:136">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
@@ -3041,6 +4935,9 @@
       <c r="E86" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="F86" s="1" t="s">
+        <v>373</v>
+      </c>
       <c r="DU86" s="1" t="s">
         <v>137</v>
       </c>
@@ -3059,8 +4956,26 @@
       <c r="DZ86" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="87" spans="1:130">
+      <c r="EA86" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="EB86" s="1">
+        <v>145</v>
+      </c>
+      <c r="EC86" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="ED86" s="1">
+        <v>40</v>
+      </c>
+      <c r="EE86" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="EF86" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:136">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -3070,6 +4985,9 @@
       <c r="E87" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="F87" s="1" t="s">
+        <v>374</v>
+      </c>
       <c r="DU87" s="1" t="s">
         <v>138</v>
       </c>
@@ -3088,8 +5006,26 @@
       <c r="DZ87" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="88" spans="1:130">
+      <c r="EA87" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="EB87" s="1">
+        <v>141</v>
+      </c>
+      <c r="EC87" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="ED87" s="1">
+        <v>40</v>
+      </c>
+      <c r="EE87" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="EF87" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:136">
       <c r="DU88" s="1" t="s">
         <v>139</v>
       </c>
@@ -3108,8 +5044,26 @@
       <c r="DZ88" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="89" spans="1:130">
+      <c r="EA88" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="EB88" s="1">
+        <v>143</v>
+      </c>
+      <c r="EC88" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="ED88" s="1">
+        <v>39</v>
+      </c>
+      <c r="EE88" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="EF88" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:136">
       <c r="A89" s="1" t="s">
         <v>216</v>
       </c>
@@ -3125,6 +5079,9 @@
       <c r="E89" s="1" t="s">
         <v>218</v>
       </c>
+      <c r="F89" s="1" t="s">
+        <v>375</v>
+      </c>
       <c r="DU89" s="1" t="s">
         <v>114</v>
       </c>
@@ -3143,8 +5100,26 @@
       <c r="DZ89" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="90" spans="1:130">
+      <c r="EA89" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="EB89" s="1">
+        <v>133</v>
+      </c>
+      <c r="EC89" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="ED89" s="1">
+        <v>38</v>
+      </c>
+      <c r="EE89" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="EF89" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:136">
       <c r="DU90" s="1" t="s">
         <v>140</v>
       </c>
@@ -3163,8 +5138,26 @@
       <c r="DZ90" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="91" spans="1:130">
+      <c r="EA90" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="EB90" s="1">
+        <v>137</v>
+      </c>
+      <c r="EC90" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="ED90" s="1">
+        <v>39</v>
+      </c>
+      <c r="EE90" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="EF90" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:136">
       <c r="A91" s="1" t="s">
         <v>216</v>
       </c>
@@ -3180,6 +5173,9 @@
       <c r="E91" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="F91" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="DU91" s="1" t="s">
         <v>141</v>
       </c>
@@ -3198,8 +5194,26 @@
       <c r="DZ91" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="92" spans="1:130">
+      <c r="EA91" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="EB91" s="1">
+        <v>193</v>
+      </c>
+      <c r="EC91" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="ED91" s="1">
+        <v>37</v>
+      </c>
+      <c r="EE91" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="EF91" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:136">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3209,6 +5223,9 @@
       <c r="E92" s="1" t="s">
         <v>224</v>
       </c>
+      <c r="F92" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="DU92" s="1" t="s">
         <v>142</v>
       </c>
@@ -3227,8 +5244,26 @@
       <c r="DZ92" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="93" spans="1:130">
+      <c r="EA92" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="EB92" s="1">
+        <v>146</v>
+      </c>
+      <c r="EC92" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="ED92" s="1">
+        <v>37</v>
+      </c>
+      <c r="EE92" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="EF92" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:136">
       <c r="DU93" s="1" t="s">
         <v>143</v>
       </c>
@@ -3247,8 +5282,26 @@
       <c r="DZ93" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="94" spans="1:130">
+      <c r="EA93" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="EB93" s="1">
+        <v>129</v>
+      </c>
+      <c r="EC93" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="ED93" s="1">
+        <v>36</v>
+      </c>
+      <c r="EE93" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="EF93" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:136">
       <c r="DU94" s="1" t="s">
         <v>144</v>
       </c>
@@ -3267,8 +5320,26 @@
       <c r="DZ94" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="95" spans="1:130">
+      <c r="EA94" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="EB94" s="1">
+        <v>144</v>
+      </c>
+      <c r="EC94" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="ED94" s="1">
+        <v>38</v>
+      </c>
+      <c r="EE94" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="EF94" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:136">
       <c r="DU95" s="1" t="s">
         <v>145</v>
       </c>
@@ -3281,8 +5352,26 @@
       <c r="DZ95" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="96" spans="1:130">
+      <c r="EA95" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="EB95" s="1">
+        <v>144</v>
+      </c>
+      <c r="EC95" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="ED95" s="1">
+        <v>37</v>
+      </c>
+      <c r="EE95" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="EF95" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:136">
       <c r="DU96" s="1" t="s">
         <v>146</v>
       </c>
@@ -3295,21 +5384,547 @@
       <c r="DZ96" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="97" spans="129:130">
+      <c r="EA96" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="EB96" s="1">
+        <v>134</v>
+      </c>
+      <c r="EC96" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="ED96" s="1">
+        <v>36</v>
+      </c>
+      <c r="EE96" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="EF96" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="129:134">
       <c r="DY97" s="1" t="s">
         <v>207</v>
       </c>
       <c r="DZ97" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="98" spans="129:130">
+      <c r="EA97" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="EB97" s="1">
+        <v>192</v>
+      </c>
+      <c r="EC97" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="ED97" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="129:134">
       <c r="DY98" s="1" t="s">
         <v>187</v>
       </c>
       <c r="DZ98" s="1">
         <v>18</v>
+      </c>
+      <c r="EA98" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="EB98" s="1">
+        <v>138</v>
+      </c>
+      <c r="EC98" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="ED98" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="129:134">
+      <c r="EA99" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="EB99" s="1">
+        <v>131</v>
+      </c>
+      <c r="EC99" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="ED99" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="129:134">
+      <c r="EA100" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="EB100" s="1">
+        <v>133</v>
+      </c>
+      <c r="EC100" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="ED100" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="129:134">
+      <c r="EA101" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="EB101" s="1">
+        <v>200</v>
+      </c>
+      <c r="EC101" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="ED101" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="129:134">
+      <c r="EA102" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="EB102" s="1">
+        <v>144</v>
+      </c>
+      <c r="EC102" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="ED102" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="103" spans="129:134">
+      <c r="EA103" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="EB103" s="1">
+        <v>152</v>
+      </c>
+      <c r="EC103" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="ED103" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="104" spans="129:134">
+      <c r="EA104" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="EB104" s="1">
+        <v>136</v>
+      </c>
+      <c r="EC104" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="ED104" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="105" spans="129:134">
+      <c r="EA105" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="EB105" s="1">
+        <v>146</v>
+      </c>
+      <c r="EC105" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="ED105" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106" spans="129:134">
+      <c r="EA106" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="EB106" s="1">
+        <v>151</v>
+      </c>
+      <c r="EC106" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="ED106" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="107" spans="129:134">
+      <c r="EA107" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="EB107" s="1">
+        <v>145</v>
+      </c>
+      <c r="EC107" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="ED107" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="129:134">
+      <c r="EA108" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="EB108" s="1">
+        <v>141</v>
+      </c>
+      <c r="EC108" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="ED108" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="129:134">
+      <c r="EA109" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="EB109" s="1">
+        <v>133</v>
+      </c>
+      <c r="EC109" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="ED109" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="129:134">
+      <c r="EA110" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="EB110" s="1">
+        <v>147</v>
+      </c>
+      <c r="EC110" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="ED110" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="129:134">
+      <c r="EA111" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="EB111" s="1">
+        <v>152</v>
+      </c>
+      <c r="EC111" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="ED111" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="112" spans="129:134">
+      <c r="EA112" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="EB112" s="1">
+        <v>153</v>
+      </c>
+      <c r="EC112" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="ED112" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="131:134">
+      <c r="EA113" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="EB113" s="1">
+        <v>141</v>
+      </c>
+      <c r="EC113" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="ED113" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="131:134">
+      <c r="EA114" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="EB114" s="1">
+        <v>139</v>
+      </c>
+      <c r="EC114" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="ED114" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" spans="131:134">
+      <c r="EA115" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="EB115" s="1">
+        <v>139</v>
+      </c>
+      <c r="EC115" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="ED115" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="116" spans="131:134">
+      <c r="EA116" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="EB116" s="1">
+        <v>195</v>
+      </c>
+      <c r="EC116" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="ED116" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="117" spans="131:134">
+      <c r="EA117" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="EB117" s="1">
+        <v>197</v>
+      </c>
+      <c r="EC117" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="ED117" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118" spans="131:134">
+      <c r="EA118" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="EB118" s="1">
+        <v>132</v>
+      </c>
+      <c r="EC118" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="ED118" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="119" spans="131:134">
+      <c r="EA119" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="EB119" s="1">
+        <v>135</v>
+      </c>
+      <c r="EC119" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="ED119" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="120" spans="131:134">
+      <c r="EA120" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="EB120" s="1">
+        <v>144</v>
+      </c>
+      <c r="EC120" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="ED120" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="121" spans="131:134">
+      <c r="EA121" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="EB121" s="1">
+        <v>157</v>
+      </c>
+      <c r="EC121" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="ED121" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" spans="131:134">
+      <c r="EA122" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="EB122" s="1">
+        <v>131</v>
+      </c>
+      <c r="EC122" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="ED122" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="123" spans="131:134">
+      <c r="EA123" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="EB123" s="1">
+        <v>134</v>
+      </c>
+      <c r="EC123" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="ED123" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="124" spans="131:134">
+      <c r="EA124" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="EB124" s="1">
+        <v>150</v>
+      </c>
+      <c r="EC124" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="ED124" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="125" spans="131:134">
+      <c r="EA125" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="EB125" s="1">
+        <v>198</v>
+      </c>
+      <c r="EC125" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="ED125" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="126" spans="131:134">
+      <c r="EA126" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="EB126" s="1">
+        <v>146</v>
+      </c>
+      <c r="EC126" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="ED126" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="131:134">
+      <c r="EA127" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="EB127" s="1">
+        <v>147</v>
+      </c>
+      <c r="EC127" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="ED127" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128" spans="131:134">
+      <c r="EA128" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="EB128" s="1">
+        <v>154</v>
+      </c>
+      <c r="EC128" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="ED128" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="129" spans="133:134">
+      <c r="EC129" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="ED129" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="130" spans="133:134">
+      <c r="EC130" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="ED130" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="131" spans="133:134">
+      <c r="EC131" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="ED131" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="132" spans="133:134">
+      <c r="EC132" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="ED132" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="133:134">
+      <c r="EC133" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="ED133" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="134" spans="133:134">
+      <c r="EC134" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="ED134" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="135" spans="133:134">
+      <c r="EC135" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="ED135" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="136" spans="133:134">
+      <c r="EC136" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="ED136" s="1">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- a64fx compilation fixes
</commit_message>
<xml_diff>
--- a/output/arch_comparison.xlsx
+++ b/output/arch_comparison.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="456">
   <si>
     <t>intel_xeon_6140</t>
   </si>
@@ -1148,6 +1148,240 @@
   </si>
   <si>
     <t xml:space="preserve">49.426875 MTEPS </t>
+  </si>
+  <si>
+    <t>a64fx</t>
+  </si>
+  <si>
+    <t>85.0 GFLOP/s</t>
+  </si>
+  <si>
+    <t>2.1 GFLOP/s</t>
+  </si>
+  <si>
+    <t>0.1%</t>
+  </si>
+  <si>
+    <t>15039682539.7 GFLOP/s</t>
+  </si>
+  <si>
+    <t>222546353.1%</t>
+  </si>
+  <si>
+    <t>39.6 GFLOP/s</t>
+  </si>
+  <si>
+    <t>0.6%</t>
+  </si>
+  <si>
+    <t>100.5 GFLOP/s</t>
+  </si>
+  <si>
+    <t>95.8%</t>
+  </si>
+  <si>
+    <t>89.3 GFLOP/s</t>
+  </si>
+  <si>
+    <t>85.1%</t>
+  </si>
+  <si>
+    <t>8.4 GFLOP/s</t>
+  </si>
+  <si>
+    <t>8.0%</t>
+  </si>
+  <si>
+    <t>30.8 GFLOP/s</t>
+  </si>
+  <si>
+    <t>29.3%</t>
+  </si>
+  <si>
+    <t>4.2 GFLOP/s</t>
+  </si>
+  <si>
+    <t>4.0%</t>
+  </si>
+  <si>
+    <t>78.3 GB/s</t>
+  </si>
+  <si>
+    <t>2080671328.7 GB/s</t>
+  </si>
+  <si>
+    <t>15394135.3%</t>
+  </si>
+  <si>
+    <t>1135753846.2 GB/s</t>
+  </si>
+  <si>
+    <t>8403032.3%</t>
+  </si>
+  <si>
+    <t>1169887179.5 GB/s</t>
+  </si>
+  <si>
+    <t>8655572.5%</t>
+  </si>
+  <si>
+    <t>556.5 GB/s</t>
+  </si>
+  <si>
+    <t>8.2%</t>
+  </si>
+  <si>
+    <t>233.3 GB/s</t>
+  </si>
+  <si>
+    <t>3.5%</t>
+  </si>
+  <si>
+    <t>544.2 GB/s</t>
+  </si>
+  <si>
+    <t>53.1%</t>
+  </si>
+  <si>
+    <t>499.9 GB/s</t>
+  </si>
+  <si>
+    <t>48.8%</t>
+  </si>
+  <si>
+    <t>622.9 GB/s</t>
+  </si>
+  <si>
+    <t>60.8%</t>
+  </si>
+  <si>
+    <t>556.6 GB/s</t>
+  </si>
+  <si>
+    <t>54.4%</t>
+  </si>
+  <si>
+    <t>618.2 GB/s</t>
+  </si>
+  <si>
+    <t>60.4%</t>
+  </si>
+  <si>
+    <t>768.0 GB/s</t>
+  </si>
+  <si>
+    <t>75.0%</t>
+  </si>
+  <si>
+    <t>899.3 GB/s</t>
+  </si>
+  <si>
+    <t>87.8%</t>
+  </si>
+  <si>
+    <t>147.2 GB/s</t>
+  </si>
+  <si>
+    <t>133.4 GB/s</t>
+  </si>
+  <si>
+    <t>502.0 GB/s</t>
+  </si>
+  <si>
+    <t>358.9 GB/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">236.66522 GB/s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">506.235898 GB/s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.553286 MTEPS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.13583 GB/s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">240.282022 GB/s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">61.463833 MTEPS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.284649 GB/s </t>
+  </si>
+  <si>
+    <t>914MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.636382 GB/s </t>
+  </si>
+  <si>
+    <t>114MB</t>
+  </si>
+  <si>
+    <t>164MB</t>
+  </si>
+  <si>
+    <t>214MB</t>
+  </si>
+  <si>
+    <t>264MB</t>
+  </si>
+  <si>
+    <t>314MB</t>
+  </si>
+  <si>
+    <t>364MB</t>
+  </si>
+  <si>
+    <t>414MB</t>
+  </si>
+  <si>
+    <t>464MB</t>
+  </si>
+  <si>
+    <t>514MB</t>
+  </si>
+  <si>
+    <t>564MB</t>
+  </si>
+  <si>
+    <t>614MB</t>
+  </si>
+  <si>
+    <t>664MB</t>
+  </si>
+  <si>
+    <t>714MB</t>
+  </si>
+  <si>
+    <t>764MB</t>
+  </si>
+  <si>
+    <t>814MB</t>
+  </si>
+  <si>
+    <t>864MB</t>
+  </si>
+  <si>
+    <t>964MB</t>
+  </si>
+  <si>
+    <t>1014MB</t>
+  </si>
+  <si>
+    <t>8.1 GB/s</t>
+  </si>
+  <si>
+    <t>0.8%</t>
+  </si>
+  <si>
+    <t>8.2 GB/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 MTEPS </t>
   </si>
 </sst>
 </file>
@@ -1232,7 +1466,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="9F8511"/>
+                <a:srgbClr val="61231E"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1458,7 +1692,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="E6DA22"/>
+                <a:srgbClr val="14B2F6"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1862,6 +2096,232 @@
                 </c:pt>
                 <c:pt idx="63">
                   <c:v>154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>a64fx</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="5CD772"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'main_stats'!$EG$65:$EG$128</c:f>
+              <c:strCache>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>1KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2KB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3KB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4KB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5KB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6KB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7KB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8KB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9KB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10KB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11KB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12KB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13KB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14KB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15KB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16KB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17KB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18KB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19KB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20KB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21KB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22KB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23KB</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24KB</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25KB</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26KB</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27KB</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28KB</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29KB</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30KB</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31KB</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'main_stats'!$EH$65:$EH$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>340</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1947,7 +2407,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="556652"/>
+                <a:srgbClr val="F95267"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -2119,7 +2579,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="D1E2EC"/>
+                <a:srgbClr val="2936E7"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -2529,6 +2989,232 @@
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>a64fx</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="3FBC79"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'main_stats'!$EI$72:$EI$136</c:f>
+              <c:strCache>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>64KB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2MB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3MB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4MB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5MB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6MB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7MB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8MB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9MB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10MB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11MB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12MB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13MB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14MB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15MB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19MB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20MB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21MB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22MB</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23MB</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24MB</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25MB</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26MB</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27MB</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28MB</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29MB</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30MB</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'main_stats'!$EJ$72:$EJ$136</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="65"/>
+                <c:pt idx="0">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2614,7 +3300,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="226A4A"/>
+                <a:srgbClr val="E12412"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -2768,7 +3454,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="DD9DC2"/>
+                <a:srgbClr val="9D01D4"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -2896,6 +3582,160 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>a64fx</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFE91"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'main_stats'!$EK$79:$EK$98</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>64MB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114MB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164MB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>214MB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>264MB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>314MB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>364MB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>414MB</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>464MB</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>514MB</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>564MB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>614MB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>664MB</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>714MB</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>764MB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>814MB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>864MB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>914MB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>964MB</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1014MB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'main_stats'!$EL$79:$EL$98</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3326,7 +4166,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:EF136"/>
+  <dimension ref="A1:EL136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3338,17 +4178,21 @@
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3367,8 +4211,11 @@
       <c r="F2" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3381,8 +4228,11 @@
       <c r="F3" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -3395,8 +4245,11 @@
       <c r="F4" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3409,8 +4262,11 @@
       <c r="F5" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G5" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -3429,8 +4285,11 @@
       <c r="F7" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3443,8 +4302,11 @@
       <c r="F8" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G8" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -3463,8 +4325,11 @@
       <c r="F10" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -3477,8 +4342,11 @@
       <c r="F11" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G11" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -3497,8 +4365,11 @@
       <c r="F13" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -3511,8 +4382,11 @@
       <c r="F14" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G14" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -3531,8 +4405,11 @@
       <c r="F16" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -3545,8 +4422,11 @@
       <c r="F17" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G17" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -3565,8 +4445,11 @@
       <c r="F19" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -3579,8 +4462,11 @@
       <c r="F20" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G20" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -3599,8 +4485,11 @@
       <c r="F22" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3613,8 +4502,11 @@
       <c r="F23" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G23" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -3633,8 +4525,11 @@
       <c r="F25" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3647,8 +4542,11 @@
       <c r="F26" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G26" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
         <v>45</v>
       </c>
@@ -3667,8 +4565,11 @@
       <c r="F28" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3681,8 +4582,11 @@
       <c r="F29" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
@@ -3697,8 +4601,11 @@
       <c r="F30" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3711,8 +4618,11 @@
       <c r="F31" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -3727,8 +4637,11 @@
       <c r="F32" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3741,8 +4654,11 @@
       <c r="F33" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -3757,8 +4673,11 @@
       <c r="F34" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3771,8 +4690,11 @@
       <c r="F35" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G35" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -3791,8 +4713,11 @@
       <c r="F37" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3805,8 +4730,11 @@
       <c r="F38" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3819,13 +4747,16 @@
       <c r="F39" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
         <v>69</v>
       </c>
@@ -3844,8 +4775,11 @@
       <c r="F41" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3858,8 +4792,11 @@
       <c r="F42" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G42" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
         <v>73</v>
       </c>
@@ -3878,8 +4815,11 @@
       <c r="F44" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3892,8 +4832,11 @@
       <c r="F45" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
@@ -3908,8 +4851,11 @@
       <c r="F46" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3922,8 +4868,11 @@
       <c r="F47" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
@@ -3938,8 +4887,11 @@
       <c r="F48" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3952,8 +4904,11 @@
       <c r="F49" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -3968,8 +4923,11 @@
       <c r="F50" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3982,8 +4940,11 @@
       <c r="F51" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
@@ -3998,8 +4959,11 @@
       <c r="F52" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -4012,8 +4976,11 @@
       <c r="F53" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
@@ -4028,8 +4995,11 @@
       <c r="F54" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -4042,8 +5012,11 @@
       <c r="F55" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G55" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
         <v>92</v>
       </c>
@@ -4062,8 +5035,11 @@
       <c r="F57" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -4076,8 +5052,11 @@
       <c r="F58" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G58" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
         <v>96</v>
       </c>
@@ -4096,8 +5075,11 @@
       <c r="F60" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
@@ -4112,8 +5094,11 @@
       <c r="F61" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -4128,8 +5113,11 @@
       <c r="F62" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
@@ -4144,12 +5132,15 @@
       <c r="F63" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="1:136">
+    <row r="65" spans="1:142">
       <c r="A65" s="1" t="s">
         <v>107</v>
       </c>
@@ -4168,6 +5159,9 @@
       <c r="F65" s="1" t="s">
         <v>273</v>
       </c>
+      <c r="G65" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="DU65" s="1" t="s">
         <v>117</v>
       </c>
@@ -4180,8 +5174,14 @@
       <c r="EB65" s="1">
         <v>153</v>
       </c>
-    </row>
-    <row r="66" spans="1:136">
+      <c r="EG65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="EH65" s="1">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="66" spans="1:142">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4194,6 +5194,9 @@
       <c r="F66" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="G66" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="DU66" s="1" t="s">
         <v>118</v>
       </c>
@@ -4206,8 +5209,14 @@
       <c r="EB66" s="1">
         <v>144</v>
       </c>
-    </row>
-    <row r="67" spans="1:136">
+      <c r="EG66" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="EH66" s="1">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:142">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4220,6 +5229,9 @@
       <c r="F67" s="1" t="s">
         <v>274</v>
       </c>
+      <c r="G67" s="1" t="s">
+        <v>426</v>
+      </c>
       <c r="DU67" s="1" t="s">
         <v>119</v>
       </c>
@@ -4232,8 +5244,14 @@
       <c r="EB67" s="1">
         <v>132</v>
       </c>
-    </row>
-    <row r="68" spans="1:136">
+      <c r="EG67" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="EH67" s="1">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="68" spans="1:142">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4246,6 +5264,9 @@
       <c r="F68" s="1" t="s">
         <v>275</v>
       </c>
+      <c r="G68" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="DU68" s="1" t="s">
         <v>120</v>
       </c>
@@ -4258,8 +5279,14 @@
       <c r="EB68" s="1">
         <v>141</v>
       </c>
-    </row>
-    <row r="69" spans="1:136">
+      <c r="EG68" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="EH68" s="1">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="69" spans="1:142">
       <c r="DU69" s="1" t="s">
         <v>121</v>
       </c>
@@ -4272,8 +5299,14 @@
       <c r="EB69" s="1">
         <v>198</v>
       </c>
-    </row>
-    <row r="70" spans="1:136">
+      <c r="EG69" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="EH69" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="70" spans="1:142">
       <c r="A70" s="1" t="s">
         <v>147</v>
       </c>
@@ -4292,6 +5325,9 @@
       <c r="F70" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="G70" s="1" t="s">
+        <v>427</v>
+      </c>
       <c r="DU70" s="1" t="s">
         <v>122</v>
       </c>
@@ -4304,8 +5340,14 @@
       <c r="EB70" s="1">
         <v>158</v>
       </c>
-    </row>
-    <row r="71" spans="1:136">
+      <c r="EG70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="EH70" s="1">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="71" spans="1:142">
       <c r="DU71" s="1" t="s">
         <v>123</v>
       </c>
@@ -4318,8 +5360,14 @@
       <c r="EB71" s="1">
         <v>146</v>
       </c>
-    </row>
-    <row r="72" spans="1:136">
+      <c r="EG71" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="EH71" s="1">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="72" spans="1:142">
       <c r="A72" s="1" t="s">
         <v>152</v>
       </c>
@@ -4338,6 +5386,9 @@
       <c r="F72" s="1" t="s">
         <v>308</v>
       </c>
+      <c r="G72" s="1" t="s">
+        <v>428</v>
+      </c>
       <c r="DU72" s="1" t="s">
         <v>124</v>
       </c>
@@ -4362,8 +5413,20 @@
       <c r="ED72" s="1">
         <v>109</v>
       </c>
-    </row>
-    <row r="73" spans="1:136">
+      <c r="EG72" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="EH72" s="1">
+        <v>301</v>
+      </c>
+      <c r="EI72" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="EJ72" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:142">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4376,6 +5439,9 @@
       <c r="F73" s="1" t="s">
         <v>309</v>
       </c>
+      <c r="G73" s="1" t="s">
+        <v>318</v>
+      </c>
       <c r="DU73" s="1" t="s">
         <v>116</v>
       </c>
@@ -4400,8 +5466,20 @@
       <c r="ED73" s="1">
         <v>83</v>
       </c>
-    </row>
-    <row r="74" spans="1:136">
+      <c r="EG73" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="EH73" s="1">
+        <v>321</v>
+      </c>
+      <c r="EI73" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="EJ73" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:142">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4414,6 +5492,9 @@
       <c r="F74" s="1" t="s">
         <v>310</v>
       </c>
+      <c r="G74" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="DU74" s="1" t="s">
         <v>125</v>
       </c>
@@ -4438,8 +5519,20 @@
       <c r="ED74" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="75" spans="1:136">
+      <c r="EG74" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="EH74" s="1">
+        <v>330</v>
+      </c>
+      <c r="EI74" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="EJ74" s="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" spans="1:142">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4452,6 +5545,9 @@
       <c r="F75" s="1" t="s">
         <v>311</v>
       </c>
+      <c r="G75" s="1" t="s">
+        <v>306</v>
+      </c>
       <c r="DU75" s="1" t="s">
         <v>126</v>
       </c>
@@ -4476,8 +5572,20 @@
       <c r="ED75" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="76" spans="1:136">
+      <c r="EG75" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="EH75" s="1">
+        <v>341</v>
+      </c>
+      <c r="EI75" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="EJ75" s="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:142">
       <c r="DU76" s="1" t="s">
         <v>127</v>
       </c>
@@ -4502,8 +5610,20 @@
       <c r="ED76" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="77" spans="1:136">
+      <c r="EG76" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="EH76" s="1">
+        <v>506</v>
+      </c>
+      <c r="EI76" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="EJ76" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:142">
       <c r="A77" s="1" t="s">
         <v>179</v>
       </c>
@@ -4522,6 +5642,9 @@
       <c r="F77" s="1" t="s">
         <v>350</v>
       </c>
+      <c r="G77" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="DU77" s="1" t="s">
         <v>128</v>
       </c>
@@ -4546,8 +5669,20 @@
       <c r="ED77" s="1">
         <v>63</v>
       </c>
-    </row>
-    <row r="78" spans="1:136">
+      <c r="EG77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="EH77" s="1">
+        <v>375</v>
+      </c>
+      <c r="EI77" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="EJ77" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:142">
       <c r="DU78" s="1" t="s">
         <v>129</v>
       </c>
@@ -4572,8 +5707,20 @@
       <c r="ED78" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="79" spans="1:136">
+      <c r="EG78" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="EH78" s="1">
+        <v>334</v>
+      </c>
+      <c r="EI78" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="EJ78" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="1:142">
       <c r="A79" s="1" t="s">
         <v>183</v>
       </c>
@@ -4592,6 +5739,9 @@
       <c r="F79" s="1" t="s">
         <v>351</v>
       </c>
+      <c r="G79" s="1" t="s">
+        <v>431</v>
+      </c>
       <c r="DU79" s="1" t="s">
         <v>130</v>
       </c>
@@ -4628,8 +5778,26 @@
       <c r="EF79" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="80" spans="1:136">
+      <c r="EG79" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="EH79" s="1">
+        <v>334</v>
+      </c>
+      <c r="EI79" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="EJ79" s="1">
+        <v>64</v>
+      </c>
+      <c r="EK79" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="EL79" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:142">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4642,6 +5810,9 @@
       <c r="F80" s="1" t="s">
         <v>352</v>
       </c>
+      <c r="G80" s="1" t="s">
+        <v>432</v>
+      </c>
       <c r="DU80" s="1" t="s">
         <v>131</v>
       </c>
@@ -4678,8 +5849,26 @@
       <c r="EF80" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="81" spans="1:136">
+      <c r="EG80" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="EH80" s="1">
+        <v>314</v>
+      </c>
+      <c r="EI80" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EJ80" s="1">
+        <v>57</v>
+      </c>
+      <c r="EK80" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="EL80" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:142">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4692,6 +5881,9 @@
       <c r="F81" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="G81" s="1" t="s">
+        <v>433</v>
+      </c>
       <c r="DU81" s="1" t="s">
         <v>132</v>
       </c>
@@ -4728,8 +5920,26 @@
       <c r="EF81" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="82" spans="1:136">
+      <c r="EG81" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="EH81" s="1">
+        <v>321</v>
+      </c>
+      <c r="EI81" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EJ81" s="1">
+        <v>48</v>
+      </c>
+      <c r="EK81" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="EL81" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:142">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4742,6 +5952,9 @@
       <c r="F82" s="1" t="s">
         <v>354</v>
       </c>
+      <c r="G82" s="1" t="s">
+        <v>348</v>
+      </c>
       <c r="DU82" s="1" t="s">
         <v>133</v>
       </c>
@@ -4778,8 +5991,26 @@
       <c r="EF82" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="83" spans="1:136">
+      <c r="EG82" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="EH82" s="1">
+        <v>313</v>
+      </c>
+      <c r="EI82" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EJ82" s="1">
+        <v>46</v>
+      </c>
+      <c r="EK82" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="EL82" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:142">
       <c r="DU83" s="1" t="s">
         <v>134</v>
       </c>
@@ -4816,8 +6047,26 @@
       <c r="EF83" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="84" spans="1:136">
+      <c r="EG83" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="EH83" s="1">
+        <v>335</v>
+      </c>
+      <c r="EI83" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="EJ83" s="1">
+        <v>45</v>
+      </c>
+      <c r="EK83" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="EL83" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:142">
       <c r="A84" s="1" t="s">
         <v>208</v>
       </c>
@@ -4836,6 +6085,9 @@
       <c r="F84" s="1" t="s">
         <v>371</v>
       </c>
+      <c r="G84" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="DU84" s="1" t="s">
         <v>135</v>
       </c>
@@ -4872,8 +6124,26 @@
       <c r="EF84" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="85" spans="1:136">
+      <c r="EG84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="EH84" s="1">
+        <v>327</v>
+      </c>
+      <c r="EI84" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="EJ84" s="1">
+        <v>41</v>
+      </c>
+      <c r="EK84" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="EL84" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:142">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4886,6 +6156,9 @@
       <c r="F85" s="1" t="s">
         <v>372</v>
       </c>
+      <c r="G85" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="DU85" s="1" t="s">
         <v>136</v>
       </c>
@@ -4922,8 +6195,26 @@
       <c r="EF85" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="86" spans="1:136">
+      <c r="EG85" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EH85" s="1">
+        <v>332</v>
+      </c>
+      <c r="EI85" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EJ85" s="1">
+        <v>38</v>
+      </c>
+      <c r="EK85" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="EL85" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:142">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
@@ -4938,6 +6229,9 @@
       <c r="F86" s="1" t="s">
         <v>373</v>
       </c>
+      <c r="G86" s="1" t="s">
+        <v>454</v>
+      </c>
       <c r="DU86" s="1" t="s">
         <v>137</v>
       </c>
@@ -4974,8 +6268,26 @@
       <c r="EF86" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="87" spans="1:136">
+      <c r="EG86" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH86" s="1">
+        <v>304</v>
+      </c>
+      <c r="EI86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="EJ86" s="1">
+        <v>40</v>
+      </c>
+      <c r="EK86" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="EL86" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:142">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -4988,6 +6300,9 @@
       <c r="F87" s="1" t="s">
         <v>374</v>
       </c>
+      <c r="G87" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="DU87" s="1" t="s">
         <v>138</v>
       </c>
@@ -5024,8 +6339,26 @@
       <c r="EF87" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="88" spans="1:136">
+      <c r="EG87" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="EH87" s="1">
+        <v>346</v>
+      </c>
+      <c r="EI87" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="EJ87" s="1">
+        <v>36</v>
+      </c>
+      <c r="EK87" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="EL87" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:142">
       <c r="DU88" s="1" t="s">
         <v>139</v>
       </c>
@@ -5062,8 +6395,26 @@
       <c r="EF88" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="89" spans="1:136">
+      <c r="EG88" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="EH88" s="1">
+        <v>327</v>
+      </c>
+      <c r="EI88" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="EJ88" s="1">
+        <v>38</v>
+      </c>
+      <c r="EK88" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="EL88" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:142">
       <c r="A89" s="1" t="s">
         <v>216</v>
       </c>
@@ -5082,6 +6433,9 @@
       <c r="F89" s="1" t="s">
         <v>375</v>
       </c>
+      <c r="G89" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="DU89" s="1" t="s">
         <v>114</v>
       </c>
@@ -5118,8 +6472,26 @@
       <c r="EF89" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="90" spans="1:136">
+      <c r="EG89" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="EH89" s="1">
+        <v>299</v>
+      </c>
+      <c r="EI89" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="EJ89" s="1">
+        <v>35</v>
+      </c>
+      <c r="EK89" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="EL89" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:142">
       <c r="DU90" s="1" t="s">
         <v>140</v>
       </c>
@@ -5156,8 +6528,26 @@
       <c r="EF90" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="91" spans="1:136">
+      <c r="EG90" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="EH90" s="1">
+        <v>353</v>
+      </c>
+      <c r="EI90" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="EJ90" s="1">
+        <v>33</v>
+      </c>
+      <c r="EK90" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="EL90" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:142">
       <c r="A91" s="1" t="s">
         <v>216</v>
       </c>
@@ -5176,6 +6566,9 @@
       <c r="F91" s="1" t="s">
         <v>376</v>
       </c>
+      <c r="G91" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="DU91" s="1" t="s">
         <v>141</v>
       </c>
@@ -5212,8 +6605,26 @@
       <c r="EF91" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="92" spans="1:136">
+      <c r="EG91" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="EH91" s="1">
+        <v>327</v>
+      </c>
+      <c r="EI91" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="EJ91" s="1">
+        <v>34</v>
+      </c>
+      <c r="EK91" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="EL91" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:142">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -5226,6 +6637,9 @@
       <c r="F92" s="1" t="s">
         <v>377</v>
       </c>
+      <c r="G92" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="DU92" s="1" t="s">
         <v>142</v>
       </c>
@@ -5262,8 +6676,26 @@
       <c r="EF92" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="93" spans="1:136">
+      <c r="EG92" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="EH92" s="1">
+        <v>280</v>
+      </c>
+      <c r="EI92" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="EJ92" s="1">
+        <v>35</v>
+      </c>
+      <c r="EK92" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="EL92" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:142">
       <c r="DU93" s="1" t="s">
         <v>143</v>
       </c>
@@ -5300,8 +6732,26 @@
       <c r="EF93" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:136">
+      <c r="EG93" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="EH93" s="1">
+        <v>309</v>
+      </c>
+      <c r="EI93" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="EJ93" s="1">
+        <v>32</v>
+      </c>
+      <c r="EK93" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="EL93" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:142">
       <c r="DU94" s="1" t="s">
         <v>144</v>
       </c>
@@ -5338,8 +6788,26 @@
       <c r="EF94" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="95" spans="1:136">
+      <c r="EG94" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="EH94" s="1">
+        <v>236</v>
+      </c>
+      <c r="EI94" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="EJ94" s="1">
+        <v>31</v>
+      </c>
+      <c r="EK94" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="EL94" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:142">
       <c r="DU95" s="1" t="s">
         <v>145</v>
       </c>
@@ -5370,8 +6838,26 @@
       <c r="EF95" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="96" spans="1:136">
+      <c r="EG95" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="EH95" s="1">
+        <v>335</v>
+      </c>
+      <c r="EI95" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="EJ95" s="1">
+        <v>33</v>
+      </c>
+      <c r="EK95" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="EL95" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:142">
       <c r="DU96" s="1" t="s">
         <v>146</v>
       </c>
@@ -5402,8 +6888,26 @@
       <c r="EF96" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="97" spans="129:134">
+      <c r="EG96" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="EH96" s="1">
+        <v>340</v>
+      </c>
+      <c r="EI96" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="EJ96" s="1">
+        <v>33</v>
+      </c>
+      <c r="EK96" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="EL96" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="129:142">
       <c r="DY97" s="1" t="s">
         <v>207</v>
       </c>
@@ -5422,8 +6926,20 @@
       <c r="ED97" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="98" spans="129:134">
+      <c r="EI97" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="EJ97" s="1">
+        <v>32</v>
+      </c>
+      <c r="EK97" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="EL97" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="129:142">
       <c r="DY98" s="1" t="s">
         <v>187</v>
       </c>
@@ -5442,8 +6958,20 @@
       <c r="ED98" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="99" spans="129:134">
+      <c r="EI98" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="EJ98" s="1">
+        <v>31</v>
+      </c>
+      <c r="EK98" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="EL98" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="129:142">
       <c r="EA99" s="1" t="s">
         <v>278</v>
       </c>
@@ -5456,8 +6984,14 @@
       <c r="ED99" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="100" spans="129:134">
+      <c r="EI99" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="EJ99" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="129:142">
       <c r="EA100" s="1" t="s">
         <v>279</v>
       </c>
@@ -5470,8 +7004,14 @@
       <c r="ED100" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="101" spans="129:134">
+      <c r="EI100" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="EJ100" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="101" spans="129:142">
       <c r="EA101" s="1" t="s">
         <v>275</v>
       </c>
@@ -5484,8 +7024,14 @@
       <c r="ED101" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="102" spans="129:134">
+      <c r="EI101" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="EJ101" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="129:142">
       <c r="EA102" s="1" t="s">
         <v>280</v>
       </c>
@@ -5498,8 +7044,14 @@
       <c r="ED102" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="103" spans="129:134">
+      <c r="EI102" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="EJ102" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="129:142">
       <c r="EA103" s="1" t="s">
         <v>281</v>
       </c>
@@ -5512,8 +7064,14 @@
       <c r="ED103" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="104" spans="129:134">
+      <c r="EI103" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="EJ103" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="104" spans="129:142">
       <c r="EA104" s="1" t="s">
         <v>282</v>
       </c>
@@ -5527,7 +7085,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="129:134">
+    <row r="105" spans="129:142">
       <c r="EA105" s="1" t="s">
         <v>283</v>
       </c>
@@ -5541,7 +7099,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="129:134">
+    <row r="106" spans="129:142">
       <c r="EA106" s="1" t="s">
         <v>284</v>
       </c>
@@ -5555,7 +7113,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="129:134">
+    <row r="107" spans="129:142">
       <c r="EA107" s="1" t="s">
         <v>285</v>
       </c>
@@ -5569,7 +7127,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="129:134">
+    <row r="108" spans="129:142">
       <c r="EA108" s="1" t="s">
         <v>286</v>
       </c>
@@ -5583,7 +7141,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="129:134">
+    <row r="109" spans="129:142">
       <c r="EA109" s="1" t="s">
         <v>287</v>
       </c>
@@ -5597,7 +7155,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="129:134">
+    <row r="110" spans="129:142">
       <c r="EA110" s="1" t="s">
         <v>288</v>
       </c>
@@ -5611,7 +7169,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="129:134">
+    <row r="111" spans="129:142">
       <c r="EA111" s="1" t="s">
         <v>289</v>
       </c>
@@ -5625,7 +7183,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="129:134">
+    <row r="112" spans="129:142">
       <c r="EA112" s="1" t="s">
         <v>290</v>
       </c>

</xml_diff>